<commit_message>
Atualizacao dados errados tabela
</commit_message>
<xml_diff>
--- a/Ensaios/7 - MIT NOVA 15 cv (14-02-2019).xlsx
+++ b/Ensaios/7 - MIT NOVA 15 cv (14-02-2019).xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Index</t>
   </si>
@@ -48,25 +48,31 @@
     <t>Vazio Final</t>
   </si>
   <si>
+    <t>Ref (kW)</t>
+  </si>
+  <si>
+    <t>Tensao</t>
+  </si>
+  <si>
+    <t>Corrente</t>
+  </si>
+  <si>
+    <t>Potencia</t>
+  </si>
+  <si>
+    <t>Frequencia</t>
+  </si>
+  <si>
+    <t>Temperatura</t>
+  </si>
+  <si>
+    <t>Torque</t>
+  </si>
+  <si>
+    <t>Velocidade</t>
+  </si>
+  <si>
     <t>Ref</t>
-  </si>
-  <si>
-    <t>Tensao</t>
-  </si>
-  <si>
-    <t>Corrente</t>
-  </si>
-  <si>
-    <t>Potencia</t>
-  </si>
-  <si>
-    <t>Frequencia</t>
-  </si>
-  <si>
-    <t>Torque</t>
-  </si>
-  <si>
-    <t>Velocidade</t>
   </si>
 </sst>
 </file>
@@ -74,7 +80,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.00000000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -92,12 +98,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="0"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -106,21 +118,26 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -370,19 +387,19 @@
         <v>6</v>
       </c>
       <c r="B2" s="2">
-        <v>1.08</v>
+        <v>0.5965</v>
       </c>
       <c r="C2" s="2">
-        <v>1.081</v>
+        <v>0.593</v>
       </c>
       <c r="D2" s="2">
-        <v>1.08</v>
-      </c>
-      <c r="E2" s="1">
-        <v>25.0</v>
+        <v>0.587</v>
+      </c>
+      <c r="E2" s="3">
+        <v>24.8</v>
       </c>
       <c r="F2" s="3">
-        <v>25.0</v>
+        <v>24.8</v>
       </c>
     </row>
     <row r="3">
@@ -390,19 +407,19 @@
         <v>7</v>
       </c>
       <c r="B3" s="2">
-        <v>1.353</v>
+        <v>0.7505</v>
       </c>
       <c r="C3" s="2">
-        <v>1.355</v>
+        <v>0.746</v>
       </c>
       <c r="D3" s="2">
-        <v>1.35</v>
-      </c>
-      <c r="E3" s="1">
-        <v>27.0</v>
-      </c>
-      <c r="F3" s="3">
-        <v>92.8</v>
+        <v>0.746</v>
+      </c>
+      <c r="E3" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>92.81790036588802</v>
       </c>
     </row>
     <row r="4">
@@ -410,18 +427,18 @@
         <v>8</v>
       </c>
       <c r="B4" s="2">
-        <v>1.326</v>
+        <v>0.74</v>
       </c>
       <c r="C4" s="2">
-        <v>1.327</v>
+        <v>0.737</v>
       </c>
       <c r="D4" s="2">
-        <v>1.32</v>
-      </c>
-      <c r="E4" s="1">
-        <v>27.0</v>
-      </c>
-      <c r="F4" s="4">
+        <v>0.735</v>
+      </c>
+      <c r="E4" s="4">
+        <v>26.0</v>
+      </c>
+      <c r="F4" s="5">
         <v>88.36608499859278</v>
       </c>
     </row>
@@ -430,19 +447,19 @@
         <v>9</v>
       </c>
       <c r="B5" s="2">
-        <v>1.311</v>
+        <v>0.74</v>
       </c>
       <c r="C5" s="2">
-        <v>1.31</v>
+        <v>0.737</v>
       </c>
       <c r="D5" s="2">
-        <v>1.307</v>
+        <v>0.735</v>
       </c>
       <c r="E5" s="1">
         <v>27.0</v>
       </c>
-      <c r="F5" s="3">
-        <v>88.0</v>
+      <c r="F5" s="5">
+        <v>88.36608499859278</v>
       </c>
     </row>
     <row r="6">
@@ -450,18 +467,18 @@
         <v>10</v>
       </c>
       <c r="B6" s="2">
-        <v>1.311</v>
+        <v>0.7165</v>
       </c>
       <c r="C6" s="2">
-        <v>1.31</v>
+        <v>0.7125</v>
       </c>
       <c r="D6" s="2">
-        <v>1.307</v>
+        <v>0.7115</v>
       </c>
       <c r="E6" s="1">
         <v>26.0</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="5">
         <v>77.92986208837607</v>
       </c>
     </row>
@@ -502,166 +519,195 @@
       <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2">
+      <c r="A2" s="5">
         <v>16.5</v>
       </c>
-      <c r="B2" s="5">
-        <v>377.26</v>
+      <c r="B2" s="6">
+        <v>380.5</v>
       </c>
       <c r="C2" s="5">
-        <v>31.796</v>
+        <v>32.521</v>
       </c>
       <c r="D2" s="5">
-        <v>18357.0</v>
+        <v>19210.0</v>
       </c>
       <c r="E2" s="5">
-        <v>60.034</v>
+        <v>60.027</v>
       </c>
       <c r="F2" s="5">
-        <v>89.930523</v>
+        <v>90.5919926822404</v>
       </c>
       <c r="G2" s="5">
-        <v>1741.033051</v>
+        <v>91.808928</v>
+      </c>
+      <c r="H2" s="5">
+        <v>1723.020376</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2">
+      <c r="A3" s="5">
         <v>13.75</v>
       </c>
-      <c r="B3" s="5">
-        <v>378.98</v>
+      <c r="B3" s="6">
+        <v>382.48</v>
       </c>
       <c r="C3" s="5">
-        <v>26.628</v>
+        <v>26.412</v>
       </c>
       <c r="D3" s="5">
-        <v>15158.0</v>
+        <v>15580.0</v>
       </c>
       <c r="E3" s="5">
+        <v>60.02</v>
+      </c>
+      <c r="F3" s="5">
+        <v>90.5919926822404</v>
+      </c>
+      <c r="G3" s="5">
+        <v>75.24143</v>
+      </c>
+      <c r="H3" s="5">
+        <v>1740.157992</v>
+      </c>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="5">
+        <v>11.0</v>
+      </c>
+      <c r="B4" s="6">
+        <v>384.47</v>
+      </c>
+      <c r="C4" s="5">
+        <v>21.234</v>
+      </c>
+      <c r="D4" s="5">
+        <v>12342.0</v>
+      </c>
+      <c r="E4" s="5">
+        <v>59.995</v>
+      </c>
+      <c r="F4" s="5">
+        <v>90.5919926822404</v>
+      </c>
+      <c r="G4" s="5">
+        <v>59.981884</v>
+      </c>
+      <c r="H4" s="5">
+        <v>1753.885956</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5">
+        <v>8.25</v>
+      </c>
+      <c r="B5" s="6">
+        <v>386.04</v>
+      </c>
+      <c r="C5" s="5">
+        <v>16.547</v>
+      </c>
+      <c r="D5" s="5">
+        <v>9211.0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>60.012</v>
+      </c>
+      <c r="F5" s="5">
+        <v>90.5919926822404</v>
+      </c>
+      <c r="G5" s="5">
+        <v>44.739505</v>
+      </c>
+      <c r="H5" s="5">
+        <v>1767.245139</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="5">
+        <v>5.5</v>
+      </c>
+      <c r="B6" s="6">
+        <v>387.61</v>
+      </c>
+      <c r="C6" s="5">
+        <v>12.549</v>
+      </c>
+      <c r="D6" s="5">
+        <v>6263.0</v>
+      </c>
+      <c r="E6" s="5">
+        <v>60.019</v>
+      </c>
+      <c r="F6" s="5">
+        <v>90.5919926822404</v>
+      </c>
+      <c r="G6" s="5">
+        <v>29.971647</v>
+      </c>
+      <c r="H6" s="5">
+        <v>1778.9134</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5">
+        <v>2.75</v>
+      </c>
+      <c r="B7" s="6">
+        <v>389.07</v>
+      </c>
+      <c r="C7" s="5">
+        <v>9.436</v>
+      </c>
+      <c r="D7" s="5">
+        <v>3401.0</v>
+      </c>
+      <c r="E7" s="5">
         <v>60.003</v>
       </c>
-      <c r="F3" s="5">
-        <v>74.852348</v>
-      </c>
-      <c r="G3" s="5">
-        <v>1752.384848</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2">
-        <v>11.0</v>
-      </c>
-      <c r="B4" s="5">
-        <v>380.5</v>
-      </c>
-      <c r="C4" s="5">
-        <v>21.759</v>
-      </c>
-      <c r="D4" s="5">
-        <v>11979.0</v>
-      </c>
-      <c r="E4" s="5">
-        <v>60.033</v>
-      </c>
-      <c r="F4" s="5">
-        <v>59.419401</v>
-      </c>
-      <c r="G4" s="5">
-        <v>1764.491383</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2">
-        <v>8.25</v>
-      </c>
-      <c r="B5" s="5">
-        <v>381.33</v>
-      </c>
-      <c r="C5" s="5">
-        <v>17.497</v>
-      </c>
-      <c r="D5" s="5">
-        <v>8970.0</v>
-      </c>
-      <c r="E5" s="5">
-        <v>60.008</v>
-      </c>
-      <c r="F5" s="5">
-        <v>44.489094</v>
-      </c>
-      <c r="G5" s="5">
-        <v>1773.766602</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2">
-        <v>5.5</v>
-      </c>
-      <c r="B6" s="5">
-        <v>382.98</v>
-      </c>
-      <c r="C6" s="5">
-        <v>13.792</v>
-      </c>
-      <c r="D6" s="5">
-        <v>5995.0</v>
-      </c>
-      <c r="E6" s="5">
-        <v>60.024</v>
-      </c>
-      <c r="F6" s="5">
-        <v>29.392511</v>
-      </c>
-      <c r="G6" s="5">
-        <v>1783.708198</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2">
-        <v>2.75</v>
-      </c>
-      <c r="B7" s="5">
-        <v>384.53</v>
-      </c>
-      <c r="C7" s="5">
-        <v>11.203</v>
-      </c>
-      <c r="D7" s="5">
-        <v>3178.0</v>
-      </c>
-      <c r="E7" s="5">
-        <v>60.026</v>
-      </c>
       <c r="F7" s="5">
-        <v>14.826677</v>
+        <v>90.5919926822404</v>
       </c>
       <c r="G7" s="5">
-        <v>1792.294476</v>
+        <v>15.298585</v>
+      </c>
+      <c r="H7" s="5">
+        <v>1789.018542</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2">
+      <c r="A8" s="5">
         <v>0.0</v>
       </c>
-      <c r="B8" s="5">
-        <v>385.74</v>
+      <c r="B8" s="6">
+        <v>390.57</v>
       </c>
       <c r="C8" s="5">
-        <v>10.192</v>
+        <v>7.937</v>
       </c>
       <c r="D8" s="5">
-        <v>666.0</v>
+        <v>763.0</v>
       </c>
       <c r="E8" s="5">
-        <v>60.003</v>
+        <v>60.0</v>
       </c>
       <c r="F8" s="5">
-        <v>1.667006</v>
+        <v>90.5919926822404</v>
       </c>
       <c r="G8" s="5">
-        <v>1799.078505</v>
+        <v>1.577724</v>
+      </c>
+      <c r="H8" s="5">
+        <v>1798.281263</v>
       </c>
     </row>
   </sheetData>
@@ -681,7 +727,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>12</v>
@@ -697,259 +743,226 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2">
+      <c r="A2" s="5">
         <v>420.0</v>
       </c>
-      <c r="B2" s="5">
-        <v>423.89</v>
-      </c>
-      <c r="C2" s="5">
-        <v>13.1</v>
-      </c>
-      <c r="D2" s="5">
-        <v>608.0</v>
-      </c>
-      <c r="E2" s="5">
-        <v>60.046</v>
+      <c r="B2" s="6">
+        <v>424.11</v>
+      </c>
+      <c r="C2" s="6">
+        <v>9.678</v>
+      </c>
+      <c r="D2" s="6">
+        <v>604.1</v>
+      </c>
+      <c r="E2" s="7">
+        <v>60.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2">
+      <c r="A3" s="5">
         <v>380.0</v>
       </c>
-      <c r="B3" s="5">
-        <v>379.93</v>
-      </c>
-      <c r="C3" s="5">
-        <v>9.744</v>
-      </c>
-      <c r="D3" s="5">
-        <v>344.0</v>
-      </c>
-      <c r="E3" s="5">
-        <v>60.045</v>
+      <c r="B3" s="6">
+        <v>379.48</v>
+      </c>
+      <c r="C3" s="6">
+        <v>7.504</v>
+      </c>
+      <c r="D3" s="6">
+        <v>452.79999999999995</v>
+      </c>
+      <c r="E3" s="7">
+        <v>60.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2">
+      <c r="A4" s="5">
         <v>340.0</v>
       </c>
-      <c r="B4" s="5">
-        <v>334.45</v>
-      </c>
-      <c r="C4" s="5">
-        <v>7.815</v>
-      </c>
-      <c r="D4" s="5">
-        <v>242.0</v>
-      </c>
-      <c r="E4" s="5">
-        <v>60.037</v>
+      <c r="B4" s="6">
+        <v>340.37</v>
+      </c>
+      <c r="C4" s="6">
+        <v>6.387</v>
+      </c>
+      <c r="D4" s="6">
+        <v>374.90000000000003</v>
+      </c>
+      <c r="E4" s="7">
+        <v>60.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2">
+      <c r="A5" s="5">
         <v>300.0</v>
       </c>
-      <c r="B5" s="5">
-        <v>298.39</v>
-      </c>
-      <c r="C5" s="5">
-        <v>6.765</v>
-      </c>
-      <c r="D5" s="5">
-        <v>202.0</v>
-      </c>
-      <c r="E5" s="5">
-        <v>60.039</v>
+      <c r="B5" s="6">
+        <v>300.01</v>
+      </c>
+      <c r="C5" s="6">
+        <v>5.512</v>
+      </c>
+      <c r="D5" s="6">
+        <v>311.3</v>
+      </c>
+      <c r="E5" s="7">
+        <v>60.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2">
+      <c r="A6" s="5">
         <v>260.0</v>
       </c>
-      <c r="B6" s="5">
-        <v>260.85</v>
-      </c>
-      <c r="C6" s="5">
-        <v>5.785</v>
-      </c>
-      <c r="D6" s="5">
+      <c r="B6" s="6">
+        <v>259.64</v>
+      </c>
+      <c r="C6" s="6">
+        <v>4.714</v>
+      </c>
+      <c r="D6" s="6">
+        <v>270.7</v>
+      </c>
+      <c r="E6" s="7">
+        <v>60.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5">
+        <v>220.0</v>
+      </c>
+      <c r="B7" s="6">
+        <v>220.2</v>
+      </c>
+      <c r="C7" s="6">
+        <v>3.965</v>
+      </c>
+      <c r="D7" s="6">
+        <v>231.7</v>
+      </c>
+      <c r="E7" s="7">
+        <v>60.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5">
+        <v>180.0</v>
+      </c>
+      <c r="B8" s="6">
+        <v>180.75</v>
+      </c>
+      <c r="C8" s="6">
+        <v>3.272</v>
+      </c>
+      <c r="D8" s="6">
+        <v>203.5</v>
+      </c>
+      <c r="E8" s="7">
+        <v>60.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="8">
         <v>160.0</v>
       </c>
-      <c r="E6" s="5">
-        <v>60.048</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2">
-        <v>220.0</v>
-      </c>
-      <c r="B7" s="5">
-        <v>221.33</v>
-      </c>
-      <c r="C7" s="5">
-        <v>4.856</v>
-      </c>
-      <c r="D7" s="5">
-        <v>132.1</v>
-      </c>
-      <c r="E7" s="5">
-        <v>60.036</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2">
-        <v>180.0</v>
-      </c>
-      <c r="B8" s="5">
-        <v>179.28</v>
-      </c>
-      <c r="C8" s="5">
-        <v>3.856</v>
-      </c>
-      <c r="D8" s="5">
-        <v>103.9</v>
-      </c>
-      <c r="E8" s="5">
-        <v>60.068</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2">
-        <v>160.0</v>
-      </c>
-      <c r="B9" s="5">
-        <v>161.32</v>
-      </c>
-      <c r="C9" s="5">
-        <v>3.465</v>
-      </c>
-      <c r="D9" s="5">
-        <v>88.8</v>
-      </c>
-      <c r="E9" s="5">
-        <v>60.05</v>
+      <c r="B9" s="6">
+        <v>159.71</v>
+      </c>
+      <c r="C9" s="6">
+        <v>2.92</v>
+      </c>
+      <c r="D9" s="6">
+        <v>188.70000000000002</v>
+      </c>
+      <c r="E9" s="7">
+        <v>60.0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2">
+      <c r="A10" s="8">
         <v>140.0</v>
       </c>
-      <c r="B10" s="5">
-        <v>141.38</v>
-      </c>
-      <c r="C10" s="5">
-        <v>3.022</v>
-      </c>
-      <c r="D10" s="5">
-        <v>81.0</v>
-      </c>
-      <c r="E10" s="5">
-        <v>60.041</v>
+      <c r="B10" s="6">
+        <v>140.22</v>
+      </c>
+      <c r="C10" s="6">
+        <v>2.607</v>
+      </c>
+      <c r="D10" s="6">
+        <v>179.10000000000002</v>
+      </c>
+      <c r="E10" s="7">
+        <v>60.0</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2">
+      <c r="A11" s="8">
         <v>120.0</v>
       </c>
-      <c r="B11" s="5">
-        <v>120.99</v>
-      </c>
-      <c r="C11" s="5">
-        <v>2.5931</v>
-      </c>
-      <c r="D11" s="5">
-        <v>70.8</v>
-      </c>
-      <c r="E11" s="5">
-        <v>60.053</v>
+      <c r="B11" s="6">
+        <v>120.41</v>
+      </c>
+      <c r="C11" s="6">
+        <v>2.311</v>
+      </c>
+      <c r="D11" s="6">
+        <v>168.8</v>
+      </c>
+      <c r="E11" s="7">
+        <v>60.0</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2">
+      <c r="A12" s="8">
         <v>100.0</v>
       </c>
-      <c r="B12" s="5">
-        <v>101.55</v>
-      </c>
-      <c r="C12" s="5">
-        <v>2.1913</v>
-      </c>
-      <c r="D12" s="5">
-        <v>65.3</v>
-      </c>
-      <c r="E12" s="5">
-        <v>60.051</v>
+      <c r="B12" s="6">
+        <v>99.71</v>
+      </c>
+      <c r="C12" s="6">
+        <v>2.044</v>
+      </c>
+      <c r="D12" s="6">
+        <v>157.1</v>
+      </c>
+      <c r="E12" s="7">
+        <v>60.0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2">
+      <c r="A13" s="8">
         <v>80.0</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="6">
         <v>80.42</v>
       </c>
-      <c r="C13" s="5">
-        <v>1.7792</v>
-      </c>
-      <c r="D13" s="5">
-        <v>58.1</v>
-      </c>
-      <c r="E13" s="5">
-        <v>60.027</v>
+      <c r="C13" s="6">
+        <v>1.892</v>
+      </c>
+      <c r="D13" s="6">
+        <v>154.20000000000002</v>
+      </c>
+      <c r="E13" s="7">
+        <v>60.0</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="2">
-        <v>60.0</v>
-      </c>
-      <c r="B14" s="5">
-        <v>60.02</v>
-      </c>
-      <c r="C14" s="5">
-        <v>1.4087</v>
-      </c>
-      <c r="D14" s="5">
-        <v>49.4</v>
-      </c>
-      <c r="E14" s="5">
-        <v>60.031</v>
-      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
     </row>
     <row r="15">
-      <c r="A15" s="2">
-        <v>40.0</v>
-      </c>
-      <c r="B15" s="5">
-        <v>40.49</v>
-      </c>
-      <c r="C15" s="5">
-        <v>1.2039</v>
-      </c>
-      <c r="D15" s="5">
-        <v>47.059999999999995</v>
-      </c>
-      <c r="E15" s="5">
-        <v>60.067</v>
-      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
     </row>
     <row r="16">
-      <c r="A16" s="2">
-        <v>20.0</v>
-      </c>
-      <c r="B16" s="5">
-        <v>30.33</v>
-      </c>
-      <c r="C16" s="5">
-        <v>1.2897</v>
-      </c>
-      <c r="D16" s="5">
-        <v>46.910000000000004</v>
-      </c>
-      <c r="E16" s="5">
-        <v>60.081</v>
-      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>